<commit_message>
all working now :D send now to get 3 ...
</commit_message>
<xml_diff>
--- a/data/level1.xlsx
+++ b/data/level1.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7224"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7224" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="level2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -103,7 +104,156 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FFFFFF00"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0066"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FFFFFF00"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0066"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF7030A0"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF800080"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3366CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <gradientFill degree="180">
@@ -544,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD12" sqref="A1:AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1683,58 +1833,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AF12">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1744,6 +1894,1209 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="32" width="3.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1">
+        <v>0</v>
+      </c>
+      <c r="S1" s="1">
+        <v>0</v>
+      </c>
+      <c r="T1" s="1">
+        <v>0</v>
+      </c>
+      <c r="U1" s="1">
+        <v>0</v>
+      </c>
+      <c r="V1" s="1">
+        <v>0</v>
+      </c>
+      <c r="W1" s="1">
+        <v>0</v>
+      </c>
+      <c r="X1" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1">
+        <v>2</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>2</v>
+      </c>
+      <c r="U2" s="1">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1">
+        <v>2</v>
+      </c>
+      <c r="W2" s="1">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>12</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1">
+        <v>3</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1">
+        <v>4</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>2</v>
+      </c>
+      <c r="X4" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>23</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>12</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>2</v>
+      </c>
+      <c r="O6" s="1">
+        <v>3</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>2</v>
+      </c>
+      <c r="R6" s="1">
+        <v>4</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>2</v>
+      </c>
+      <c r="X6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>21</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>15</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2</v>
+      </c>
+      <c r="N8" s="1">
+        <v>2</v>
+      </c>
+      <c r="O8" s="1">
+        <v>3</v>
+      </c>
+      <c r="P8" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>2</v>
+      </c>
+      <c r="R8" s="1">
+        <v>4</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1</v>
+      </c>
+      <c r="V8" s="1">
+        <v>2</v>
+      </c>
+      <c r="W8" s="1">
+        <v>2</v>
+      </c>
+      <c r="X8" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>23</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>3</v>
+      </c>
+      <c r="P10" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2</v>
+      </c>
+      <c r="R10" s="1">
+        <v>4</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1</v>
+      </c>
+      <c r="V10" s="1">
+        <v>2</v>
+      </c>
+      <c r="W10" s="1">
+        <v>2</v>
+      </c>
+      <c r="X10" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>22</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>13</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>22</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>13</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>21</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>5</v>
+      </c>
+      <c r="M12" s="1">
+        <v>5</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5</v>
+      </c>
+      <c r="O12" s="1">
+        <v>5</v>
+      </c>
+      <c r="P12" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>5</v>
+      </c>
+      <c r="R12" s="1">
+        <v>5</v>
+      </c>
+      <c r="S12" s="1">
+        <v>21</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>5</v>
+      </c>
+      <c r="V12" s="1">
+        <v>5</v>
+      </c>
+      <c r="W12" s="1">
+        <v>5</v>
+      </c>
+      <c r="X12" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>21</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AF12">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>24</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>23</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>14</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>22</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>

</xml_diff>

<commit_message>
95% sound added, high score added, start screen added.
</commit_message>
<xml_diff>
--- a/data/level1.xlsx
+++ b/data/level1.xlsx
@@ -1898,7 +1898,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1994,9 +1994,7 @@
       <c r="AC1" s="1">
         <v>0</v>
       </c>
-      <c r="AD1" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
@@ -2088,9 +2086,7 @@
       <c r="AC2" s="1">
         <v>7</v>
       </c>
-      <c r="AD2" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
     </row>
@@ -2182,9 +2178,7 @@
       <c r="AC3" s="1">
         <v>7</v>
       </c>
-      <c r="AD3" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
     </row>
@@ -2276,9 +2270,7 @@
       <c r="AC4" s="1">
         <v>7</v>
       </c>
-      <c r="AD4" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
     </row>
@@ -2370,9 +2362,7 @@
       <c r="AC5" s="1">
         <v>7</v>
       </c>
-      <c r="AD5" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
     </row>
@@ -2464,9 +2454,7 @@
       <c r="AC6" s="1">
         <v>7</v>
       </c>
-      <c r="AD6" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
     </row>
@@ -2558,9 +2546,7 @@
       <c r="AC7" s="1">
         <v>7</v>
       </c>
-      <c r="AD7" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
     </row>
@@ -2652,9 +2638,7 @@
       <c r="AC8" s="1">
         <v>7</v>
       </c>
-      <c r="AD8" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1"/>
     </row>
@@ -2746,9 +2730,7 @@
       <c r="AC9" s="1">
         <v>7</v>
       </c>
-      <c r="AD9" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
     </row>
@@ -2840,9 +2822,7 @@
       <c r="AC10" s="1">
         <v>7</v>
       </c>
-      <c r="AD10" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1"/>
     </row>
@@ -2934,9 +2914,7 @@
       <c r="AC11" s="1">
         <v>7</v>
       </c>
-      <c r="AD11" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
@@ -3028,9 +3006,7 @@
       <c r="AC12" s="1">
         <v>5</v>
       </c>
-      <c r="AD12" s="1">
-        <v>0</v>
-      </c>
+      <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>

</xml_diff>